<commit_message>
add customers table into orders table and build related html files.
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lance\Desktop\New folder\btbc\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA652288-096E-4933-BF47-85940E764C57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BB2271-0575-4834-8B0D-A191E89F69F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="118">
   <si>
     <t>pppp</t>
   </si>
@@ -261,9 +261,6 @@
     <t>Customer Name:</t>
   </si>
   <si>
-    <t>Barossa Trading and Bottling Company Pty Ltd</t>
-  </si>
-  <si>
     <t>RUN:</t>
   </si>
   <si>
@@ -285,18 +282,6 @@
     <t>Contact Person:</t>
   </si>
   <si>
-    <t>Ethan Lin</t>
-  </si>
-  <si>
-    <t>0426546592</t>
-  </si>
-  <si>
-    <t>Bob Li</t>
-  </si>
-  <si>
-    <t>0422983978</t>
-  </si>
-  <si>
     <t>Address:</t>
   </si>
   <si>
@@ -309,12 +294,6 @@
     <t>Email:</t>
   </si>
   <si>
-    <t>production@barossatrading.com</t>
-  </si>
-  <si>
-    <t>bob@barossatrading.com</t>
-  </si>
-  <si>
     <t>Fax:</t>
   </si>
   <si>
@@ -351,10 +330,6 @@
     <t>LOSCAM</t>
   </si>
   <si>
-    <t>CAN BE</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Bottles:</t>
   </si>
   <si>
@@ -388,21 +363,12 @@
     <t>Cardboard</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>Stretch Wrap</t>
   </si>
   <si>
-    <t>Std</t>
-  </si>
-  <si>
     <t>CONT. SIZE</t>
   </si>
   <si>
-    <t>40FT</t>
-  </si>
-  <si>
     <t>Once bottled dispatch to;</t>
   </si>
   <si>
@@ -419,6 +385,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -1518,9 +1487,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1545,6 +1511,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1593,6 +1562,30 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1607,30 +1600,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2145,8 +2114,8 @@
   </sheetPr>
   <dimension ref="A1:AG123"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A24" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:G36"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
@@ -2259,54 +2228,43 @@
       <c r="P5" s="19"/>
     </row>
     <row r="6" spans="1:16" ht="14.25" customHeight="1">
-      <c r="A6" s="158" t="s">
+      <c r="A6" s="166" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="158"/>
-      <c r="C6" s="23" t="s">
-        <v>75</v>
-      </c>
+      <c r="B6" s="166"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="24"/>
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
       <c r="G6" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H6" s="190"/>
       <c r="I6" s="190"/>
       <c r="J6" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="K6" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="K6" s="26" t="s">
+      <c r="M6" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="M6" s="27" t="s">
+      <c r="N6" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="N6" s="28" t="s">
+      <c r="O6" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="O6" s="28" t="s">
+    </row>
+    <row r="7" spans="1:16" ht="14.5">
+      <c r="A7" s="166" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="14.5">
-      <c r="A7" s="158" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="158"/>
-      <c r="C7" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>86</v>
-      </c>
+      <c r="B7" s="166"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="F7" s="29"/>
       <c r="H7" s="30"/>
       <c r="J7" s="31"/>
       <c r="K7" s="31"/>
@@ -2316,22 +2274,22 @@
       <c r="O7" s="32"/>
     </row>
     <row r="8" spans="1:16" ht="13.5">
-      <c r="A8" s="158" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" s="158"/>
+      <c r="A8" s="166" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="166"/>
       <c r="C8" s="33"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
       <c r="F8" s="34"/>
       <c r="G8" s="34"/>
       <c r="H8" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I8" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="J8" s="24"/>
+        <v>84</v>
+      </c>
+      <c r="J8" s="35"/>
       <c r="K8" s="24"/>
       <c r="L8" s="31"/>
       <c r="M8" s="32"/>
@@ -2339,21 +2297,17 @@
       <c r="O8" s="32"/>
     </row>
     <row r="9" spans="1:16" ht="13">
-      <c r="A9" s="158" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="158"/>
-      <c r="C9" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="36" t="s">
-        <v>92</v>
-      </c>
+      <c r="A9" s="166" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="166"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
       <c r="H9" s="10" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
@@ -2372,17 +2326,17 @@
       <c r="O10" s="32"/>
     </row>
     <row r="11" spans="1:16" ht="13.5" customHeight="1">
-      <c r="A11" s="158" t="s">
-        <v>94</v>
-      </c>
-      <c r="B11" s="158"/>
+      <c r="A11" s="166" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="166"/>
       <c r="C11" s="39"/>
       <c r="D11" s="24"/>
       <c r="E11" s="40"/>
       <c r="F11" s="40"/>
       <c r="G11" s="24"/>
       <c r="H11" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I11" s="41"/>
       <c r="J11" s="42"/>
@@ -2416,7 +2370,7 @@
       <c r="O13" s="32"/>
     </row>
     <row r="14" spans="1:16" ht="17.149999999999999" customHeight="1">
-      <c r="A14" s="158" t="s">
+      <c r="A14" s="166" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="175"/>
@@ -2440,7 +2394,7 @@
       <c r="O14" s="32"/>
     </row>
     <row r="15" spans="1:16" ht="17.149999999999999" customHeight="1">
-      <c r="A15" s="158" t="s">
+      <c r="A15" s="166" t="s">
         <v>6</v>
       </c>
       <c r="B15" s="175"/>
@@ -2466,7 +2420,7 @@
       <c r="O15" s="32"/>
     </row>
     <row r="16" spans="1:16" ht="17.149999999999999" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="166" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="175"/>
@@ -2487,7 +2441,7 @@
       <c r="O16" s="32"/>
     </row>
     <row r="17" spans="1:33" ht="17.149999999999999" customHeight="1" thickBot="1">
-      <c r="A17" s="158" t="s">
+      <c r="A17" s="166" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="175"/>
@@ -2516,7 +2470,7 @@
       <c r="O17" s="32"/>
     </row>
     <row r="18" spans="1:33" ht="17.149999999999999" customHeight="1" thickTop="1">
-      <c r="A18" s="158" t="s">
+      <c r="A18" s="166" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="175"/>
@@ -2542,7 +2496,7 @@
       <c r="O18" s="32"/>
     </row>
     <row r="19" spans="1:33" ht="17.149999999999999" customHeight="1">
-      <c r="A19" s="158" t="s">
+      <c r="A19" s="166" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="175"/>
@@ -2552,7 +2506,7 @@
         <v>20</v>
       </c>
       <c r="F19" s="180"/>
-      <c r="G19" s="160"/>
+      <c r="G19" s="168"/>
       <c r="H19" s="59" t="s">
         <v>21</v>
       </c>
@@ -2566,17 +2520,17 @@
       <c r="O19" s="32"/>
     </row>
     <row r="20" spans="1:33" ht="17.149999999999999" customHeight="1">
-      <c r="A20" s="158" t="s">
+      <c r="A20" s="166" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="158"/>
+      <c r="B20" s="166"/>
       <c r="C20" s="62"/>
       <c r="D20" s="49"/>
       <c r="E20" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="159"/>
-      <c r="G20" s="160"/>
+      <c r="F20" s="167"/>
+      <c r="G20" s="168"/>
       <c r="H20" s="171"/>
       <c r="I20" s="172"/>
       <c r="J20" s="63"/>
@@ -2586,17 +2540,17 @@
       <c r="O20" s="32"/>
     </row>
     <row r="21" spans="1:33" ht="17.149999999999999" customHeight="1">
-      <c r="A21" s="158" t="s">
+      <c r="A21" s="166" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="158"/>
+      <c r="B21" s="166"/>
       <c r="C21" s="62"/>
       <c r="D21" s="58"/>
       <c r="E21" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="159"/>
-      <c r="G21" s="160"/>
+      <c r="F21" s="167"/>
+      <c r="G21" s="168"/>
       <c r="H21" s="173"/>
       <c r="I21" s="174"/>
       <c r="J21" s="63"/>
@@ -2606,15 +2560,15 @@
       <c r="O21" s="32"/>
     </row>
     <row r="22" spans="1:33" ht="18" customHeight="1">
-      <c r="A22" s="158" t="s">
+      <c r="A22" s="166" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="158"/>
+      <c r="B22" s="166"/>
       <c r="C22" s="57"/>
       <c r="D22" s="49"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="159"/>
-      <c r="G22" s="160"/>
+      <c r="F22" s="167"/>
+      <c r="G22" s="168"/>
       <c r="H22" s="3"/>
       <c r="I22" s="4"/>
       <c r="J22" s="42"/>
@@ -2624,15 +2578,15 @@
       <c r="O22" s="16"/>
     </row>
     <row r="23" spans="1:33" ht="18" customHeight="1">
-      <c r="A23" s="158" t="s">
+      <c r="A23" s="166" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="158"/>
+      <c r="B23" s="166"/>
       <c r="C23" s="57"/>
       <c r="D23" s="49"/>
       <c r="E23" s="24"/>
-      <c r="F23" s="159"/>
-      <c r="G23" s="160"/>
+      <c r="F23" s="167"/>
+      <c r="G23" s="168"/>
       <c r="H23" s="64" t="s">
         <v>28</v>
       </c>
@@ -2644,17 +2598,17 @@
       <c r="O23" s="16"/>
     </row>
     <row r="24" spans="1:33" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A24" s="161" t="s">
+      <c r="A24" s="169" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="161"/>
+      <c r="B24" s="169"/>
       <c r="C24" s="57"/>
-      <c r="D24" s="162" t="s">
+      <c r="D24" s="170" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="162"/>
-      <c r="F24" s="159"/>
-      <c r="G24" s="160"/>
+      <c r="E24" s="170"/>
+      <c r="F24" s="167"/>
+      <c r="G24" s="168"/>
       <c r="H24" s="5" t="s">
         <v>31</v>
       </c>
@@ -2665,15 +2619,15 @@
       <c r="O24" s="16"/>
     </row>
     <row r="25" spans="1:33">
-      <c r="A25" s="163" t="s">
+      <c r="A25" s="158" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="164"/>
+      <c r="B25" s="159"/>
       <c r="C25" s="66"/>
       <c r="D25" s="66"/>
       <c r="E25" s="66"/>
-      <c r="F25" s="167"/>
-      <c r="G25" s="168"/>
+      <c r="F25" s="162"/>
+      <c r="G25" s="163"/>
       <c r="H25" s="67"/>
       <c r="I25" s="68"/>
       <c r="J25" s="69"/>
@@ -2683,8 +2637,8 @@
       <c r="O25" s="70"/>
     </row>
     <row r="26" spans="1:33" ht="13" thickBot="1">
-      <c r="A26" s="165"/>
-      <c r="B26" s="166"/>
+      <c r="A26" s="160"/>
+      <c r="B26" s="161"/>
       <c r="C26" s="71" t="s">
         <v>33</v>
       </c>
@@ -2694,10 +2648,10 @@
       <c r="E26" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="169" t="s">
+      <c r="F26" s="164" t="s">
         <v>36</v>
       </c>
-      <c r="G26" s="170"/>
+      <c r="G26" s="165"/>
       <c r="H26" s="73" t="s">
         <v>37</v>
       </c>
@@ -2752,20 +2706,17 @@
       <c r="AG29" s="16"/>
     </row>
     <row r="30" spans="1:33" ht="18" customHeight="1">
-      <c r="A30" s="137" t="s">
+      <c r="A30" s="136" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="138"/>
+      <c r="B30" s="137"/>
       <c r="C30" s="83"/>
       <c r="D30" s="151"/>
       <c r="E30" s="152"/>
       <c r="F30" s="152"/>
       <c r="G30" s="153"/>
       <c r="H30" s="7"/>
-      <c r="I30" s="7">
-        <f>$C$16*$H$14</f>
-        <v>10656</v>
-      </c>
+      <c r="I30" s="7"/>
       <c r="J30" s="69"/>
       <c r="K30" s="42"/>
       <c r="M30" s="70">
@@ -2780,27 +2731,24 @@
         <v>44</v>
       </c>
       <c r="R30" s="84" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="AE30" s="70"/>
       <c r="AF30" s="70"/>
       <c r="AG30" s="70"/>
     </row>
     <row r="31" spans="1:33" ht="18" customHeight="1">
-      <c r="A31" s="137" t="s">
+      <c r="A31" s="136" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="138"/>
+      <c r="B31" s="137"/>
       <c r="C31" s="83"/>
       <c r="D31" s="151"/>
       <c r="E31" s="152"/>
       <c r="F31" s="152"/>
       <c r="G31" s="153"/>
       <c r="H31" s="7"/>
-      <c r="I31" s="7">
-        <f>I30</f>
-        <v>10656</v>
-      </c>
+      <c r="I31" s="7"/>
       <c r="J31" s="69"/>
       <c r="K31" s="42"/>
       <c r="M31" s="70">
@@ -2813,27 +2761,24 @@
         <v>44</v>
       </c>
       <c r="R31" s="84" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="AE31" s="70"/>
       <c r="AF31" s="70"/>
       <c r="AG31" s="70"/>
     </row>
     <row r="32" spans="1:33" ht="18" customHeight="1">
-      <c r="A32" s="137" t="s">
+      <c r="A32" s="136" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="138"/>
+      <c r="B32" s="137"/>
       <c r="C32" s="85"/>
       <c r="D32" s="151"/>
       <c r="E32" s="152"/>
       <c r="F32" s="152"/>
       <c r="G32" s="153"/>
       <c r="H32" s="7"/>
-      <c r="I32" s="7">
-        <f>I30</f>
-        <v>10656</v>
-      </c>
+      <c r="I32" s="7"/>
       <c r="J32" s="69"/>
       <c r="K32" s="42"/>
       <c r="M32" s="70">
@@ -2846,7 +2791,7 @@
         <v>44</v>
       </c>
       <c r="R32" s="84" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="AE32" s="70">
         <f>H14</f>
@@ -2861,20 +2806,17 @@
       </c>
     </row>
     <row r="33" spans="1:33" ht="18" customHeight="1">
-      <c r="A33" s="137" t="s">
+      <c r="A33" s="136" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="138"/>
+      <c r="B33" s="137"/>
       <c r="C33" s="85"/>
       <c r="D33" s="151"/>
       <c r="E33" s="152"/>
       <c r="F33" s="152"/>
       <c r="G33" s="153"/>
       <c r="H33" s="7"/>
-      <c r="I33" s="7">
-        <f>I30+300</f>
-        <v>10956</v>
-      </c>
+      <c r="I33" s="7"/>
       <c r="J33" s="69"/>
       <c r="K33" s="42"/>
       <c r="M33" s="70">
@@ -2886,7 +2828,7 @@
       </c>
       <c r="O33" s="82"/>
       <c r="Q33" s="13" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="R33" s="86"/>
       <c r="AE33" s="70">
@@ -2902,30 +2844,27 @@
       </c>
     </row>
     <row r="34" spans="1:33" ht="18" customHeight="1">
-      <c r="A34" s="137" t="s">
+      <c r="A34" s="136" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="138"/>
+      <c r="B34" s="137"/>
       <c r="C34" s="85"/>
       <c r="D34" s="151"/>
       <c r="E34" s="152"/>
       <c r="F34" s="152"/>
       <c r="G34" s="153"/>
       <c r="H34" s="7"/>
-      <c r="I34" s="7">
-        <f>$C$16*$H$14+300</f>
-        <v>10956</v>
-      </c>
+      <c r="I34" s="7"/>
       <c r="J34" s="69"/>
       <c r="K34" s="42"/>
       <c r="M34" s="70"/>
       <c r="N34" s="82"/>
       <c r="O34" s="82"/>
       <c r="Q34" s="13" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="R34" s="87" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="AA34" s="70">
         <v>6</v>
@@ -2960,10 +2899,7 @@
       <c r="F35" s="146"/>
       <c r="G35" s="147"/>
       <c r="H35" s="7"/>
-      <c r="I35" s="7">
-        <f>C16</f>
-        <v>888</v>
-      </c>
+      <c r="I35" s="7"/>
       <c r="J35" s="69"/>
       <c r="K35" s="42"/>
       <c r="M35" s="70">
@@ -2975,7 +2911,7 @@
         <v>44</v>
       </c>
       <c r="R35" s="84" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="AA35" s="70">
         <f>AA34</f>
@@ -2993,20 +2929,17 @@
       <c r="AG35" s="82"/>
     </row>
     <row r="36" spans="1:33" ht="18" customHeight="1">
-      <c r="A36" s="137" t="s">
+      <c r="A36" s="136" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="138"/>
+      <c r="B36" s="137"/>
       <c r="C36" s="85"/>
       <c r="D36" s="145"/>
       <c r="E36" s="146"/>
       <c r="F36" s="146"/>
       <c r="G36" s="147"/>
       <c r="H36" s="7"/>
-      <c r="I36" s="7">
-        <f>C16</f>
-        <v>888</v>
-      </c>
+      <c r="I36" s="7"/>
       <c r="J36" s="69"/>
       <c r="K36" s="42"/>
       <c r="M36" s="70">
@@ -3018,7 +2951,7 @@
         <v>44</v>
       </c>
       <c r="R36" s="84" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="AA36" s="70">
         <v>6</v>
@@ -3035,10 +2968,10 @@
       <c r="AG36" s="82"/>
     </row>
     <row r="37" spans="1:33" ht="18" customHeight="1">
-      <c r="A37" s="137" t="s">
+      <c r="A37" s="136" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="138"/>
+      <c r="B37" s="137"/>
       <c r="C37" s="8">
         <f>C20</f>
         <v>0</v>
@@ -3051,10 +2984,7 @@
       <c r="F37" s="149"/>
       <c r="G37" s="150"/>
       <c r="H37" s="90"/>
-      <c r="I37" s="91">
-        <f>C17</f>
-        <v>8080.7999999999993</v>
-      </c>
+      <c r="I37" s="91"/>
       <c r="J37" s="69"/>
       <c r="K37" s="42"/>
       <c r="M37" s="70">
@@ -3084,15 +3014,15 @@
       </c>
     </row>
     <row r="38" spans="1:33" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A38" s="137" t="s">
+      <c r="A38" s="136" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="138"/>
+      <c r="B38" s="137"/>
       <c r="C38" s="9"/>
-      <c r="D38" s="139"/>
-      <c r="E38" s="140"/>
-      <c r="F38" s="140"/>
-      <c r="G38" s="141"/>
+      <c r="D38" s="138"/>
+      <c r="E38" s="139"/>
+      <c r="F38" s="139"/>
+      <c r="G38" s="140"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="69"/>
@@ -3101,10 +3031,10 @@
       <c r="N38" s="70"/>
       <c r="O38" s="70"/>
       <c r="P38" s="13" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="Q38" s="13" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="AA38" s="70"/>
       <c r="AB38" s="82"/>
@@ -3121,11 +3051,11 @@
       </c>
     </row>
     <row r="39" spans="1:33" ht="14.9" customHeight="1">
-      <c r="A39" s="142" t="s">
+      <c r="A39" s="141" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="142"/>
-      <c r="C39" s="142"/>
+      <c r="B39" s="141"/>
+      <c r="C39" s="141"/>
       <c r="D39" s="93">
         <f>C11</f>
         <v>0</v>
@@ -3352,24 +3282,24 @@
     </row>
     <row r="48" spans="1:33" ht="15.5">
       <c r="A48" s="129" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B48" s="129"/>
-      <c r="C48" s="135" t="s">
-        <v>104</v>
-      </c>
-      <c r="D48" s="135"/>
+      <c r="C48" s="142" t="s">
+        <v>97</v>
+      </c>
+      <c r="D48" s="142"/>
       <c r="E48" s="103" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="G48" s="104" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="I48" s="105" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="J48" s="42"/>
       <c r="K48" s="42"/>
@@ -3385,16 +3315,14 @@
     </row>
     <row r="49" spans="1:33" ht="15.5">
       <c r="A49" s="129" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B49" s="129"/>
-      <c r="C49" s="106">
-        <v>14</v>
-      </c>
+      <c r="C49" s="106"/>
       <c r="D49" s="106"/>
       <c r="E49" s="103"/>
       <c r="H49" s="10" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="I49" s="107"/>
       <c r="J49" s="42"/>
@@ -3411,16 +3339,14 @@
     </row>
     <row r="50" spans="1:33" ht="15.5">
       <c r="A50" s="129" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B50" s="129"/>
-      <c r="C50" s="106">
-        <v>5</v>
-      </c>
+      <c r="C50" s="106"/>
       <c r="D50" s="106"/>
       <c r="E50" s="103"/>
       <c r="H50" s="10" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="I50" s="107"/>
       <c r="J50" s="42"/>
@@ -3434,13 +3360,10 @@
     </row>
     <row r="51" spans="1:33" ht="15.5">
       <c r="A51" s="129" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B51" s="129"/>
-      <c r="C51" s="106">
-        <f>C50*C49</f>
-        <v>70</v>
-      </c>
+      <c r="C51" s="106"/>
       <c r="D51" s="106"/>
       <c r="E51" s="103"/>
       <c r="I51" s="108"/>
@@ -3458,27 +3381,25 @@
     </row>
     <row r="52" spans="1:33" ht="15.5">
       <c r="A52" s="129" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B52" s="129"/>
-      <c r="C52" s="136" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" s="136"/>
+      <c r="C52" s="135"/>
+      <c r="D52" s="135"/>
       <c r="G52" s="104" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="H52" s="10" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="I52" s="109" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="J52" s="42"/>
       <c r="K52" s="42"/>
       <c r="M52" s="70">
         <f>C51</f>
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="N52" s="70"/>
       <c r="O52" s="82"/>
@@ -3491,15 +3412,13 @@
     </row>
     <row r="53" spans="1:33" ht="15.5">
       <c r="A53" s="132" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B53" s="132"/>
-      <c r="C53" s="133" t="s">
-        <v>117</v>
-      </c>
+      <c r="C53" s="133"/>
       <c r="D53" s="133"/>
       <c r="H53" s="10" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="I53" s="109"/>
       <c r="J53" s="42"/>
@@ -3512,24 +3431,22 @@
       <c r="AC53" s="70"/>
       <c r="AE53" s="70">
         <f>C51</f>
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="AF53" s="70">
         <v>2.5</v>
       </c>
-      <c r="AG53" s="70">
+      <c r="AG53" s="70" t="e">
         <f>AF53/AE53</f>
-        <v>3.5714285714285712E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="54" spans="1:33" ht="15.5">
       <c r="A54" s="129" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B54" s="129"/>
-      <c r="C54" s="133" t="s">
-        <v>119</v>
-      </c>
+      <c r="C54" s="133"/>
       <c r="D54" s="133"/>
       <c r="H54" s="10"/>
       <c r="I54" s="108"/>
@@ -3537,7 +3454,7 @@
       <c r="K54" s="42"/>
       <c r="M54" s="70">
         <f>M52</f>
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="N54" s="70"/>
       <c r="O54" s="82"/>
@@ -3550,12 +3467,10 @@
     </row>
     <row r="55" spans="1:33" ht="15.5">
       <c r="A55" s="129" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B55" s="129"/>
-      <c r="C55" s="134" t="s">
-        <v>121</v>
-      </c>
+      <c r="C55" s="134"/>
       <c r="D55" s="134"/>
       <c r="H55" s="10"/>
       <c r="I55" s="108"/>
@@ -3573,7 +3488,7 @@
     </row>
     <row r="56" spans="1:33" ht="13">
       <c r="A56" s="129" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B56" s="129"/>
       <c r="C56" s="130"/>
@@ -3596,7 +3511,7 @@
     </row>
     <row r="57" spans="1:33" ht="13">
       <c r="A57" s="129" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B57" s="129"/>
       <c r="C57" s="34"/>
@@ -3625,7 +3540,7 @@
     <row r="58" spans="1:33">
       <c r="K58" s="31"/>
       <c r="M58" s="110" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="N58" s="111"/>
       <c r="O58" s="82"/>
@@ -3638,14 +3553,14 @@
     </row>
     <row r="59" spans="1:33" ht="15.75" customHeight="1">
       <c r="A59" s="127" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B59" s="127"/>
       <c r="C59" s="131"/>
       <c r="D59" s="131"/>
       <c r="E59" s="131"/>
       <c r="F59" s="127" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="G59" s="127"/>
       <c r="H59" s="112"/>
@@ -3653,7 +3568,7 @@
       <c r="J59" s="113"/>
       <c r="K59" s="114"/>
       <c r="M59" s="70" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="N59" s="70"/>
       <c r="O59" s="82"/>
@@ -3900,13 +3815,11 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{1D358C24-35CA-40BB-ACDD-BC91EF39A3A7}"/>
-    <hyperlink ref="C9" r:id="rId2" xr:uid="{B3D219F8-B7FF-494C-A4DE-C4F2DE8161A8}"/>
-    <hyperlink ref="E9" r:id="rId3" xr:uid="{E983F691-F31A-4E0B-ABFF-390A13BBDA1B}"/>
   </hyperlinks>
   <pageMargins left="0.23622047244094499" right="0.23622047244094499" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="82" fitToHeight="2" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" scale="83" fitToHeight="2" orientation="portrait" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add more columns in orders table.
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lance\Desktop\New folder\btbc\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BB2271-0575-4834-8B0D-A191E89F69F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F406CD8-3118-4BE4-A725-925CC72C140F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="114">
   <si>
     <t>pppp</t>
   </si>
@@ -60,12 +60,6 @@
     <t>Run Length</t>
   </si>
   <si>
-    <t>Run Out Wine</t>
-  </si>
-  <si>
-    <t>Req'd by:</t>
-  </si>
-  <si>
     <t>Total Cases</t>
   </si>
   <si>
@@ -75,9 +69,6 @@
     <t>COA</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>Samples</t>
   </si>
   <si>
@@ -219,9 +210,6 @@
     <t>Neck:</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>mm from base of cap center to front label</t>
   </si>
   <si>
@@ -327,18 +315,12 @@
     <t>Pallet type</t>
   </si>
   <si>
-    <t>LOSCAM</t>
-  </si>
-  <si>
     <t>Bottles:</t>
   </si>
   <si>
     <t>Upright</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Cartons/lLayer</t>
   </si>
   <si>
@@ -388,15 +370,22 @@
   </si>
   <si>
     <t>`</t>
+  </si>
+  <si>
+    <t>Delivered By:</t>
+  </si>
+  <si>
+    <t>Required By:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="d/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="51">
     <font>
@@ -1183,7 +1172,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="191">
+  <cellXfs count="192">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1628,7 +1617,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1672,31 +1664,31 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="166" formatCode=";;;"/>
+      <numFmt numFmtId="167" formatCode=";;;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode=";;;"/>
+      <numFmt numFmtId="167" formatCode=";;;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode=";;;"/>
+      <numFmt numFmtId="167" formatCode=";;;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode=";;;"/>
+      <numFmt numFmtId="167" formatCode=";;;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode=";;;"/>
+      <numFmt numFmtId="167" formatCode=";;;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode=";;;"/>
+      <numFmt numFmtId="167" formatCode=";;;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode=";;;"/>
+      <numFmt numFmtId="167" formatCode=";;;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode=";;;"/>
+      <numFmt numFmtId="167" formatCode=";;;"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode=";;;"/>
+      <numFmt numFmtId="167" formatCode=";;;"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -2115,7 +2107,7 @@
   <dimension ref="A1:AG123"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
@@ -2141,11 +2133,11 @@
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
       <c r="G1" s="14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H1" s="12"/>
       <c r="I1" s="15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
@@ -2164,7 +2156,7 @@
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
       <c r="H2" s="15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I2" s="19"/>
       <c r="J2" s="19"/>
@@ -2179,7 +2171,7 @@
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="19"/>
@@ -2198,10 +2190,10 @@
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
       <c r="I4" s="19"/>
-      <c r="J4" s="187" t="s">
-        <v>72</v>
-      </c>
-      <c r="K4" s="187"/>
+      <c r="J4" s="188" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="188"/>
       <c r="L4" s="19"/>
       <c r="M4" s="17"/>
       <c r="N4" s="20"/>
@@ -2212,15 +2204,15 @@
       <c r="A5" s="18"/>
       <c r="B5" s="18"/>
       <c r="C5" s="22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
-      <c r="H5" s="189"/>
-      <c r="I5" s="189"/>
-      <c r="J5" s="188"/>
-      <c r="K5" s="188"/>
+      <c r="H5" s="190"/>
+      <c r="I5" s="190"/>
+      <c r="J5" s="189"/>
+      <c r="K5" s="189"/>
       <c r="L5" s="19"/>
       <c r="M5" s="17"/>
       <c r="N5" s="20"/>
@@ -2229,7 +2221,7 @@
     </row>
     <row r="6" spans="1:16" ht="14.25" customHeight="1">
       <c r="A6" s="166" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B6" s="166"/>
       <c r="C6" s="23"/>
@@ -2237,29 +2229,29 @@
       <c r="E6" s="24"/>
       <c r="F6" s="24"/>
       <c r="G6" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" s="191"/>
+      <c r="I6" s="191"/>
+      <c r="J6" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="M6" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="N6" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="H6" s="190"/>
-      <c r="I6" s="190"/>
-      <c r="J6" s="26" t="s">
+      <c r="O6" s="28" t="s">
         <v>76</v>
-      </c>
-      <c r="K6" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="M6" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="N6" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="O6" s="28" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="14.5">
       <c r="A7" s="166" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B7" s="166"/>
       <c r="C7" s="23"/>
@@ -2275,7 +2267,7 @@
     </row>
     <row r="8" spans="1:16" ht="13.5">
       <c r="A8" s="166" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B8" s="166"/>
       <c r="C8" s="33"/>
@@ -2284,10 +2276,10 @@
       <c r="F8" s="34"/>
       <c r="G8" s="34"/>
       <c r="H8" s="10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I8" s="35" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J8" s="35"/>
       <c r="K8" s="24"/>
@@ -2298,7 +2290,7 @@
     </row>
     <row r="9" spans="1:16" ht="13">
       <c r="A9" s="166" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B9" s="166"/>
       <c r="C9" s="36"/>
@@ -2307,7 +2299,7 @@
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
       <c r="H9" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
@@ -2327,7 +2319,7 @@
     </row>
     <row r="11" spans="1:16" ht="13.5" customHeight="1">
       <c r="A11" s="166" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B11" s="166"/>
       <c r="C11" s="39"/>
@@ -2336,7 +2328,7 @@
       <c r="F11" s="40"/>
       <c r="G11" s="24"/>
       <c r="H11" s="10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I11" s="41"/>
       <c r="J11" s="42"/>
@@ -2402,15 +2394,13 @@
         <v>0</v>
       </c>
       <c r="D15" s="49"/>
-      <c r="E15" s="181" t="s">
+      <c r="E15" s="182" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="183" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="184"/>
+      <c r="F15" s="184"/>
+      <c r="G15" s="185"/>
       <c r="H15" s="50" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="42"/>
@@ -2421,7 +2411,7 @@
     </row>
     <row r="16" spans="1:16" ht="17.149999999999999" customHeight="1">
       <c r="A16" s="166" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16" s="175"/>
       <c r="C16" s="48">
@@ -2429,10 +2419,12 @@
         <v>888</v>
       </c>
       <c r="D16" s="49"/>
-      <c r="E16" s="182"/>
-      <c r="F16" s="185"/>
-      <c r="G16" s="186"/>
-      <c r="H16" s="51"/>
+      <c r="E16" s="183"/>
+      <c r="F16" s="186"/>
+      <c r="G16" s="187"/>
+      <c r="H16" s="51" t="s">
+        <v>112</v>
+      </c>
       <c r="I16" s="52"/>
       <c r="J16" s="42"/>
       <c r="K16" s="42"/>
@@ -2442,7 +2434,7 @@
     </row>
     <row r="17" spans="1:33" ht="17.149999999999999" customHeight="1" thickBot="1">
       <c r="A17" s="166" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17" s="175"/>
       <c r="C17" s="53">
@@ -2451,17 +2443,15 @@
       </c>
       <c r="D17" s="54"/>
       <c r="E17" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="176" t="s">
-        <v>13</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F17" s="176"/>
       <c r="G17" s="177"/>
       <c r="H17" s="55" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I17" s="56" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J17" s="42"/>
       <c r="K17" s="42"/>
@@ -2471,20 +2461,18 @@
     </row>
     <row r="18" spans="1:33" ht="17.149999999999999" customHeight="1" thickTop="1">
       <c r="A18" s="166" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18" s="175"/>
       <c r="C18" s="57"/>
       <c r="D18" s="58"/>
       <c r="E18" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="178" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F18" s="178"/>
       <c r="G18" s="179"/>
       <c r="H18" s="59" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I18" s="60">
         <v>2</v>
@@ -2497,18 +2485,18 @@
     </row>
     <row r="19" spans="1:33" ht="17.149999999999999" customHeight="1">
       <c r="A19" s="166" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B19" s="175"/>
       <c r="C19" s="57"/>
       <c r="D19" s="49"/>
       <c r="E19" s="61" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F19" s="180"/>
-      <c r="G19" s="168"/>
+      <c r="G19" s="181"/>
       <c r="H19" s="59" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I19" s="60">
         <v>1</v>
@@ -2521,13 +2509,13 @@
     </row>
     <row r="20" spans="1:33" ht="17.149999999999999" customHeight="1">
       <c r="A20" s="166" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B20" s="166"/>
       <c r="C20" s="62"/>
       <c r="D20" s="49"/>
       <c r="E20" s="43" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F20" s="167"/>
       <c r="G20" s="168"/>
@@ -2541,13 +2529,13 @@
     </row>
     <row r="21" spans="1:33" ht="17.149999999999999" customHeight="1">
       <c r="A21" s="166" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B21" s="166"/>
       <c r="C21" s="62"/>
       <c r="D21" s="58"/>
       <c r="E21" s="43" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F21" s="167"/>
       <c r="G21" s="168"/>
@@ -2561,7 +2549,7 @@
     </row>
     <row r="22" spans="1:33" ht="18" customHeight="1">
       <c r="A22" s="166" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B22" s="166"/>
       <c r="C22" s="57"/>
@@ -2579,7 +2567,7 @@
     </row>
     <row r="23" spans="1:33" ht="18" customHeight="1">
       <c r="A23" s="166" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B23" s="166"/>
       <c r="C23" s="57"/>
@@ -2588,7 +2576,7 @@
       <c r="F23" s="167"/>
       <c r="G23" s="168"/>
       <c r="H23" s="64" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I23" s="64"/>
       <c r="J23" s="42"/>
@@ -2599,18 +2587,18 @@
     </row>
     <row r="24" spans="1:33" ht="24.75" customHeight="1" thickBot="1">
       <c r="A24" s="169" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B24" s="169"/>
       <c r="C24" s="57"/>
       <c r="D24" s="170" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E24" s="170"/>
       <c r="F24" s="167"/>
       <c r="G24" s="168"/>
       <c r="H24" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I24" s="6"/>
       <c r="J24" s="65"/>
@@ -2620,7 +2608,7 @@
     </row>
     <row r="25" spans="1:33">
       <c r="A25" s="158" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B25" s="159"/>
       <c r="C25" s="66"/>
@@ -2640,20 +2628,20 @@
       <c r="A26" s="160"/>
       <c r="B26" s="161"/>
       <c r="C26" s="71" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="72" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="164" t="s">
         <v>33</v>
-      </c>
-      <c r="D26" s="72" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" s="72" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" s="164" t="s">
-        <v>36</v>
       </c>
       <c r="G26" s="165"/>
       <c r="H26" s="73" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I26" s="74"/>
       <c r="J26" s="31"/>
@@ -2664,7 +2652,7 @@
     </row>
     <row r="27" spans="1:33" ht="15" thickBot="1">
       <c r="C27" s="75" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D27" s="76"/>
       <c r="E27" s="76"/>
@@ -2674,29 +2662,29 @@
     </row>
     <row r="28" spans="1:33" ht="13.5" thickBot="1">
       <c r="H28" s="154" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I28" s="155"/>
     </row>
     <row r="29" spans="1:33" ht="13">
       <c r="A29" s="156" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B29" s="157"/>
       <c r="C29" s="77" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D29" s="78"/>
       <c r="E29" s="79" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F29" s="79"/>
       <c r="G29" s="79"/>
       <c r="H29" s="80" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I29" s="81" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M29" s="70"/>
       <c r="N29" s="82"/>
@@ -2707,7 +2695,7 @@
     </row>
     <row r="30" spans="1:33" ht="18" customHeight="1">
       <c r="A30" s="136" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B30" s="137"/>
       <c r="C30" s="83"/>
@@ -2728,10 +2716,10 @@
       </c>
       <c r="O30" s="82"/>
       <c r="Q30" s="13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="R30" s="84" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="AE30" s="70"/>
       <c r="AF30" s="70"/>
@@ -2739,7 +2727,7 @@
     </row>
     <row r="31" spans="1:33" ht="18" customHeight="1">
       <c r="A31" s="136" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B31" s="137"/>
       <c r="C31" s="83"/>
@@ -2758,10 +2746,10 @@
       <c r="N31" s="82"/>
       <c r="O31" s="82"/>
       <c r="Q31" s="13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="R31" s="84" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="AE31" s="70"/>
       <c r="AF31" s="70"/>
@@ -2769,7 +2757,7 @@
     </row>
     <row r="32" spans="1:33" ht="18" customHeight="1">
       <c r="A32" s="136" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B32" s="137"/>
       <c r="C32" s="85"/>
@@ -2788,10 +2776,10 @@
       <c r="N32" s="82"/>
       <c r="O32" s="82"/>
       <c r="Q32" s="13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="R32" s="84" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="AE32" s="70">
         <f>H14</f>
@@ -2807,7 +2795,7 @@
     </row>
     <row r="33" spans="1:33" ht="18" customHeight="1">
       <c r="A33" s="136" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B33" s="137"/>
       <c r="C33" s="85"/>
@@ -2828,7 +2816,7 @@
       </c>
       <c r="O33" s="82"/>
       <c r="Q33" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="R33" s="86"/>
       <c r="AE33" s="70">
@@ -2845,7 +2833,7 @@
     </row>
     <row r="34" spans="1:33" ht="18" customHeight="1">
       <c r="A34" s="136" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B34" s="137"/>
       <c r="C34" s="85"/>
@@ -2861,10 +2849,10 @@
       <c r="N34" s="82"/>
       <c r="O34" s="82"/>
       <c r="Q34" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="R34" s="87" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="AA34" s="70">
         <v>6</v>
@@ -2890,7 +2878,7 @@
     </row>
     <row r="35" spans="1:33" ht="18" customHeight="1">
       <c r="A35" s="143" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B35" s="144"/>
       <c r="C35" s="88"/>
@@ -2908,10 +2896,10 @@
       <c r="N35" s="82"/>
       <c r="O35" s="82"/>
       <c r="Q35" s="13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="R35" s="84" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="AA35" s="70">
         <f>AA34</f>
@@ -2930,7 +2918,7 @@
     </row>
     <row r="36" spans="1:33" ht="18" customHeight="1">
       <c r="A36" s="136" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B36" s="137"/>
       <c r="C36" s="85"/>
@@ -2948,10 +2936,10 @@
       <c r="N36" s="82"/>
       <c r="O36" s="82"/>
       <c r="Q36" s="13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="R36" s="84" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="AA36" s="70">
         <v>6</v>
@@ -2969,7 +2957,7 @@
     </row>
     <row r="37" spans="1:33" ht="18" customHeight="1">
       <c r="A37" s="136" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B37" s="137"/>
       <c r="C37" s="8">
@@ -2996,7 +2984,7 @@
       </c>
       <c r="O37" s="82"/>
       <c r="Q37" s="13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="R37" s="92"/>
       <c r="AA37" s="70"/>
@@ -3015,7 +3003,7 @@
     </row>
     <row r="38" spans="1:33" ht="24.75" customHeight="1" thickBot="1">
       <c r="A38" s="136" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B38" s="137"/>
       <c r="C38" s="9"/>
@@ -3031,10 +3019,10 @@
       <c r="N38" s="70"/>
       <c r="O38" s="70"/>
       <c r="P38" s="13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="Q38" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="AA38" s="70"/>
       <c r="AB38" s="82"/>
@@ -3052,7 +3040,7 @@
     </row>
     <row r="39" spans="1:33" ht="14.9" customHeight="1">
       <c r="A39" s="141" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B39" s="141"/>
       <c r="C39" s="141"/>
@@ -3092,11 +3080,11 @@
     </row>
     <row r="40" spans="1:33" ht="13">
       <c r="A40" s="129" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B40" s="129"/>
       <c r="C40" s="95" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D40" s="24"/>
       <c r="J40" s="42"/>
@@ -3120,11 +3108,11 @@
     </row>
     <row r="41" spans="1:33" ht="13">
       <c r="A41" s="129" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B41" s="129"/>
       <c r="C41" s="93" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D41" s="95"/>
       <c r="E41" s="31"/>
@@ -3152,17 +3140,15 @@
     </row>
     <row r="42" spans="1:33" ht="13">
       <c r="A42" s="129" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B42" s="129"/>
       <c r="C42" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>61</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="D42" s="16"/>
       <c r="E42" s="96" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F42" s="97"/>
       <c r="J42" s="42"/>
@@ -3181,13 +3167,11 @@
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D43" s="98">
-        <v>999</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D43" s="98"/>
       <c r="E43" s="99" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F43" s="99"/>
       <c r="J43" s="42"/>
@@ -3206,13 +3190,11 @@
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D44" s="98">
-        <v>999</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D44" s="98"/>
       <c r="E44" s="99" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F44" s="99"/>
       <c r="J44" s="42"/>
@@ -3231,7 +3213,7 @@
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D45" s="100"/>
       <c r="E45" s="99"/>
@@ -3249,7 +3231,7 @@
     </row>
     <row r="46" spans="1:33" ht="13">
       <c r="A46" s="102" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B46" s="102"/>
       <c r="C46" s="16"/>
@@ -3282,25 +3264,21 @@
     </row>
     <row r="48" spans="1:33" ht="15.5">
       <c r="A48" s="129" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B48" s="129"/>
-      <c r="C48" s="142" t="s">
-        <v>97</v>
-      </c>
+      <c r="C48" s="142"/>
       <c r="D48" s="142"/>
       <c r="E48" s="103" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G48" s="104" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="I48" s="105" t="s">
-        <v>100</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="I48" s="105"/>
       <c r="J48" s="42"/>
       <c r="K48" s="42"/>
       <c r="M48" s="70"/>
@@ -3315,14 +3293,14 @@
     </row>
     <row r="49" spans="1:33" ht="15.5">
       <c r="A49" s="129" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B49" s="129"/>
       <c r="C49" s="106"/>
       <c r="D49" s="106"/>
       <c r="E49" s="103"/>
       <c r="H49" s="10" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="I49" s="107"/>
       <c r="J49" s="42"/>
@@ -3339,14 +3317,14 @@
     </row>
     <row r="50" spans="1:33" ht="15.5">
       <c r="A50" s="129" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B50" s="129"/>
       <c r="C50" s="106"/>
       <c r="D50" s="106"/>
       <c r="E50" s="103"/>
       <c r="H50" s="10" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I50" s="107"/>
       <c r="J50" s="42"/>
@@ -3360,7 +3338,7 @@
     </row>
     <row r="51" spans="1:33" ht="15.5">
       <c r="A51" s="129" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B51" s="129"/>
       <c r="C51" s="106"/>
@@ -3381,20 +3359,18 @@
     </row>
     <row r="52" spans="1:33" ht="15.5">
       <c r="A52" s="129" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B52" s="129"/>
       <c r="C52" s="135"/>
       <c r="D52" s="135"/>
       <c r="G52" s="104" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="H52" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="I52" s="109" t="s">
-        <v>100</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="I52" s="109"/>
       <c r="J52" s="42"/>
       <c r="K52" s="42"/>
       <c r="M52" s="70">
@@ -3412,13 +3388,13 @@
     </row>
     <row r="53" spans="1:33" ht="15.5">
       <c r="A53" s="132" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B53" s="132"/>
       <c r="C53" s="133"/>
       <c r="D53" s="133"/>
       <c r="H53" s="10" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="I53" s="109"/>
       <c r="J53" s="42"/>
@@ -3443,7 +3419,7 @@
     </row>
     <row r="54" spans="1:33" ht="15.5">
       <c r="A54" s="129" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B54" s="129"/>
       <c r="C54" s="133"/>
@@ -3467,7 +3443,7 @@
     </row>
     <row r="55" spans="1:33" ht="15.5">
       <c r="A55" s="129" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B55" s="129"/>
       <c r="C55" s="134"/>
@@ -3488,7 +3464,7 @@
     </row>
     <row r="56" spans="1:33" ht="13">
       <c r="A56" s="129" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B56" s="129"/>
       <c r="C56" s="130"/>
@@ -3511,7 +3487,7 @@
     </row>
     <row r="57" spans="1:33" ht="13">
       <c r="A57" s="129" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B57" s="129"/>
       <c r="C57" s="34"/>
@@ -3540,7 +3516,7 @@
     <row r="58" spans="1:33">
       <c r="K58" s="31"/>
       <c r="M58" s="110" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="N58" s="111"/>
       <c r="O58" s="82"/>
@@ -3553,14 +3529,14 @@
     </row>
     <row r="59" spans="1:33" ht="15.75" customHeight="1">
       <c r="A59" s="127" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B59" s="127"/>
       <c r="C59" s="131"/>
       <c r="D59" s="131"/>
       <c r="E59" s="131"/>
       <c r="F59" s="127" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="G59" s="127"/>
       <c r="H59" s="112"/>
@@ -3568,7 +3544,7 @@
       <c r="J59" s="113"/>
       <c r="K59" s="114"/>
       <c r="M59" s="70" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="N59" s="70"/>
       <c r="O59" s="82"/>

</xml_diff>